<commit_message>
Finished electric AOE and fire AOE
also:
Finished water gun and bubble gun
Made elemental attacks
made static electric ball
made effects for grass attack and rock attack
loaded sound assets
</commit_message>
<xml_diff>
--- a/Draft/Monster data/Monster data.xlsx
+++ b/Draft/Monster data/Monster data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="60" windowWidth="19395" windowHeight="9855"/>
+    <workbookView xWindow="600" yWindow="60" windowWidth="19395" windowHeight="9855" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Monster Data" sheetId="2" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="92">
   <si>
     <t>Blast</t>
   </si>
@@ -219,9 +219,6 @@
     <t>Attacker</t>
   </si>
   <si>
-    <t>Defencer</t>
-  </si>
-  <si>
     <t>Blows fire from its mouth, dealing fire damage</t>
   </si>
   <si>
@@ -283,6 +280,18 @@
   </si>
   <si>
     <t>Wraps itself with static charges, and crush towards the enemy, dealing Electric damage.</t>
+  </si>
+  <si>
+    <t>Defender</t>
+  </si>
+  <si>
+    <t>Stings enemy with spikes, dealing normal damage.</t>
+  </si>
+  <si>
+    <t>O</t>
+  </si>
+  <si>
+    <t>ok?</t>
   </si>
 </sst>
 </file>
@@ -691,9 +700,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A20" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="G31" sqref="G31"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A9" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -879,7 +888,7 @@
         <v>1.5</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H8" s="3" t="s">
         <v>38</v>
@@ -917,7 +926,7 @@
         <v>2.5</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H9" s="3" t="s">
         <v>38</v>
@@ -943,7 +952,7 @@
         <v>31</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>2</v>
@@ -955,7 +964,7 @@
         <v>4</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H10" s="3" t="s">
         <v>38</v>
@@ -1010,7 +1019,7 @@
         <v>36</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H13" s="3" t="s">
         <v>38</v>
@@ -1031,7 +1040,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="14" spans="1:13">
+    <row r="14" spans="1:13" ht="31.5">
       <c r="B14" s="3" t="s">
         <v>30</v>
       </c>
@@ -1048,7 +1057,7 @@
         <v>36</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>64</v>
+        <v>89</v>
       </c>
       <c r="H14" s="3" t="s">
         <v>38</v>
@@ -1086,7 +1095,7 @@
         <v>36</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H15" s="3" t="s">
         <v>38</v>
@@ -1141,7 +1150,7 @@
         <v>36</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H18" s="3" t="s">
         <v>38</v>
@@ -1167,7 +1176,7 @@
         <v>30</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>1</v>
@@ -1179,7 +1188,7 @@
         <v>36</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H19" s="3" t="s">
         <v>38</v>
@@ -1272,7 +1281,7 @@
         <v>36</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H23" s="3" t="s">
         <v>38</v>
@@ -1298,7 +1307,7 @@
         <v>30</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>2</v>
@@ -1310,7 +1319,7 @@
         <v>36</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H24" s="3" t="s">
         <v>38</v>
@@ -1336,7 +1345,7 @@
         <v>31</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>4</v>
@@ -1348,7 +1357,7 @@
         <v>36</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H25" s="3" t="s">
         <v>38</v>
@@ -1403,7 +1412,7 @@
         <v>36</v>
       </c>
       <c r="G28" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H28" s="3" t="s">
         <v>38</v>
@@ -1441,7 +1450,7 @@
         <v>36</v>
       </c>
       <c r="G29" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H29" s="3" t="s">
         <v>38</v>
@@ -1479,7 +1488,7 @@
         <v>36</v>
       </c>
       <c r="G30" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H30" s="3" t="s">
         <v>38</v>
@@ -1511,7 +1520,7 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -1523,7 +1532,7 @@
     </row>
     <row r="2" spans="1:8">
       <c r="C2" s="11" t="s">
-        <v>66</v>
+        <v>88</v>
       </c>
       <c r="D2" s="11"/>
       <c r="E2" s="11"/>
@@ -1533,7 +1542,7 @@
     </row>
     <row r="3" spans="1:8">
       <c r="C3" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>25</v>
@@ -1553,28 +1562,28 @@
     </row>
     <row r="4" spans="1:8" ht="26.25" customHeight="1">
       <c r="A4" s="10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C4">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="D4">
-        <v>1</v>
+        <v>0.6</v>
       </c>
       <c r="E4">
-        <v>1</v>
+        <v>0.6</v>
       </c>
       <c r="F4">
-        <v>1</v>
+        <v>0.6</v>
       </c>
       <c r="G4">
-        <v>1</v>
+        <v>0.6</v>
       </c>
       <c r="H4">
-        <v>1</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="26.25" customHeight="1">
@@ -1583,19 +1592,19 @@
         <v>25</v>
       </c>
       <c r="C5">
-        <v>1</v>
+        <v>0.4</v>
       </c>
       <c r="D5">
         <v>0.2</v>
       </c>
       <c r="E5">
-        <v>0.2</v>
+        <v>0.7</v>
       </c>
       <c r="F5">
-        <v>0.8</v>
+        <v>0.3</v>
       </c>
       <c r="G5">
-        <v>0.7</v>
+        <v>0.5</v>
       </c>
       <c r="H5">
         <v>0.8</v>
@@ -1607,22 +1616,22 @@
         <v>47</v>
       </c>
       <c r="C6">
-        <v>1</v>
+        <v>0.4</v>
       </c>
       <c r="D6">
-        <v>0.7</v>
+        <v>0.2</v>
       </c>
       <c r="E6">
         <v>0.2</v>
       </c>
       <c r="F6">
-        <v>0.3</v>
+        <v>0.7</v>
       </c>
       <c r="G6">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="H6">
-        <v>0.3</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="26.25" customHeight="1">
@@ -1631,22 +1640,22 @@
         <v>48</v>
       </c>
       <c r="C7">
-        <v>1</v>
+        <v>0.4</v>
       </c>
       <c r="D7">
+        <v>0.8</v>
+      </c>
+      <c r="E7">
         <v>0.3</v>
-      </c>
-      <c r="E7">
-        <v>0.7</v>
       </c>
       <c r="F7">
         <v>0.2</v>
       </c>
       <c r="G7">
-        <v>0.2</v>
+        <v>0.7</v>
       </c>
       <c r="H7">
-        <v>0.7</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="26.25" customHeight="1">
@@ -1655,22 +1664,22 @@
         <v>49</v>
       </c>
       <c r="C8">
-        <v>1</v>
+        <v>0.4</v>
       </c>
       <c r="D8">
-        <v>0.5</v>
+        <v>0.7</v>
       </c>
       <c r="E8">
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
       <c r="F8">
-        <v>0.7</v>
+        <v>0.2</v>
       </c>
       <c r="G8">
         <v>0.5</v>
       </c>
       <c r="H8">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="26.25" customHeight="1">
@@ -1679,19 +1688,19 @@
         <v>50</v>
       </c>
       <c r="C9">
-        <v>1</v>
+        <v>0.4</v>
       </c>
       <c r="D9">
         <v>0.8</v>
       </c>
       <c r="E9">
-        <v>0.8</v>
+        <v>0.3</v>
       </c>
       <c r="F9">
+        <v>0.7</v>
+      </c>
+      <c r="G9">
         <v>0.5</v>
-      </c>
-      <c r="G9">
-        <v>0.8</v>
       </c>
       <c r="H9">
         <v>0.2</v>
@@ -1708,10 +1717,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:F7"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -1723,8 +1732,11 @@
     <col min="6" max="6" width="23.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" ht="31.5" customHeight="1"/>
-    <row r="2" spans="2:6" ht="63" customHeight="1">
+    <row r="1" spans="1:6" ht="31.5" customHeight="1"/>
+    <row r="2" spans="1:6" ht="63" customHeight="1">
+      <c r="A2" t="s">
+        <v>91</v>
+      </c>
       <c r="B2" t="s">
         <v>16</v>
       </c>
@@ -1741,7 +1753,10 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="2:6" ht="31.5">
+    <row r="3" spans="1:6" ht="31.5">
+      <c r="A3" t="s">
+        <v>90</v>
+      </c>
       <c r="B3" t="s">
         <v>0</v>
       </c>
@@ -1752,13 +1767,16 @@
         <v>8</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="2:6" ht="34.5" customHeight="1">
+    <row r="4" spans="1:6" ht="34.5" customHeight="1">
+      <c r="A4" t="s">
+        <v>90</v>
+      </c>
       <c r="B4" t="s">
         <v>1</v>
       </c>
@@ -1769,13 +1787,16 @@
         <v>11</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="2:6" ht="31.5">
+    <row r="5" spans="1:6" ht="31.5">
+      <c r="A5" t="s">
+        <v>90</v>
+      </c>
       <c r="B5" t="s">
         <v>2</v>
       </c>
@@ -1792,7 +1813,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="2:6" ht="31.5">
+    <row r="6" spans="1:6" ht="31.5">
       <c r="B6" t="s">
         <v>3</v>
       </c>
@@ -1809,7 +1830,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="2:6" ht="31.5">
+    <row r="7" spans="1:6" ht="31.5">
       <c r="B7" t="s">
         <v>4</v>
       </c>
@@ -1817,7 +1838,7 @@
         <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>17</v>

</xml_diff>

<commit_message>
Finished Crush, added Sound to most attacks
</commit_message>
<xml_diff>
--- a/Draft/Monster data/Monster data.xlsx
+++ b/Draft/Monster data/Monster data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="92">
   <si>
     <t>Blast</t>
   </si>
@@ -1720,7 +1720,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -1831,6 +1831,9 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="31.5">
+      <c r="A7" t="s">
+        <v>90</v>
+      </c>
       <c r="B7" t="s">
         <v>4</v>
       </c>

</xml_diff>